<commit_message>
Add ELN-based feature selection and update analysis
Introduces src_analisi/ELN_sep.py for ElasticNet-based feature selection and model evaluation. Updates RFE_sep.py to use RandomForest for feature selection, restricts model/grid search space, and disables KNN/MLP models. Several Excel results files are renamed, added, or deleted for improved organization. Also includes updates to main_syllables.py (adds legacy MFCC code as comments) and adds new analysis/figure scripts and data files.
</commit_message>
<xml_diff>
--- a/Results/First test/results_regression_sep (MFCCs).xlsx
+++ b/Results/First test/results_regression_sep (MFCCs).xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fppie\Projects\VOC\Results\First test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mimos\Projects\VOC\Results\First test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{473CFD0E-BB53-47A4-ADCC-69FE3D3408B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC0C2D4B-7B6B-4C86-AB20-1B886A557E0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43080" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1082,35 +1082,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="AC4" sqref="AC4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="78.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="255.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="255.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="127.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.86328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1328125" customWidth="1"/>
+    <col min="5" max="5" width="11.59765625" customWidth="1"/>
+    <col min="6" max="6" width="10.265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.46484375" customWidth="1"/>
+    <col min="8" max="8" width="15.3984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.3984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="29.796875" customWidth="1"/>
     <col min="11" max="13" width="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.73046875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.86328125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.1328125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.86328125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.1328125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.265625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="12" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1178,7 +1178,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -1248,7 +1248,7 @@
         <v>1.3324003524934009</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -1318,7 +1318,7 @@
         <v>0.15719192306050836</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -1388,7 +1388,7 @@
         <v>1.2224698978484585</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1458,7 +1458,7 @@
         <v>0.256061220910897</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -1528,7 +1528,7 @@
         <v>1.2191949734058778</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1598,7 +1598,7 @@
         <v>0.27122613594902845</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -1654,7 +1654,7 @@
         <v>-0.29729729729729742</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -1710,7 +1710,7 @@
         <v>-0.29729729729729742</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -1766,7 +1766,7 @@
         <v>0.51351351351351349</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -1822,7 +1822,7 @@
         <v>0.35135135135135132</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -1878,7 +1878,7 @@
         <v>0.56756756756756754</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -1934,7 +1934,7 @@
         <v>0.2432432432432432</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -1990,7 +1990,7 @@
         <v>0.18918918918918909</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -2046,7 +2046,7 @@
         <v>0.51351351351351349</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -2102,7 +2102,7 @@
         <v>0.2432432432432432</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -2172,7 +2172,7 @@
         <v>1.3129928104845274</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -2242,7 +2242,7 @@
         <v>0.18986805844043811</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -2312,7 +2312,7 @@
         <v>1.1341600969736605</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -2382,7 +2382,7 @@
         <v>0.11696527019888123</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -2452,7 +2452,7 @@
         <v>1.2387235041302109</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -2522,7 +2522,7 @@
         <v>7.459276315683544E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>18</v>
       </c>
@@ -2578,7 +2578,7 @@
         <v>2.702702702702697E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>18</v>
       </c>
@@ -2634,7 +2634,7 @@
         <v>2.702702702702697E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>18</v>
       </c>
@@ -2690,7 +2690,7 @@
         <v>0.2432432432432432</v>
       </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>18</v>
       </c>
@@ -2746,7 +2746,7 @@
         <v>-0.18918918918918931</v>
       </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>18</v>
       </c>
@@ -2802,7 +2802,7 @@
         <v>0.29729729729729731</v>
       </c>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>18</v>
       </c>
@@ -2858,7 +2858,7 @@
         <v>0.18918918918918909</v>
       </c>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>18</v>
       </c>
@@ -2914,7 +2914,7 @@
         <v>0.35135135135135132</v>
       </c>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>18</v>
       </c>
@@ -2970,7 +2970,7 @@
         <v>0.45945945945945937</v>
       </c>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>18</v>
       </c>
@@ -3026,7 +3026,7 @@
         <v>0.29729729729729731</v>
       </c>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>18</v>
       </c>
@@ -3096,7 +3096,7 @@
         <v>1.3934194487558778</v>
       </c>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>18</v>
       </c>
@@ -3166,7 +3166,7 @@
         <v>0.19591385818483234</v>
       </c>
     </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>18</v>
       </c>
@@ -3236,7 +3236,7 @@
         <v>1.4362695690074094</v>
       </c>
     </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>18</v>
       </c>
@@ -3306,7 +3306,7 @@
         <v>0.27772238862445187</v>
       </c>
     </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>18</v>
       </c>
@@ -3376,7 +3376,7 @@
         <v>1.3446839994360897</v>
       </c>
     </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>18</v>
       </c>
@@ -3446,7 +3446,7 @@
         <v>0.178395464237639</v>
       </c>
     </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>18</v>
       </c>
@@ -3502,7 +3502,7 @@
         <v>-0.35135135135135132</v>
       </c>
     </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>18</v>
       </c>
@@ -3558,7 +3558,7 @@
         <v>-8.1081081081081141E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>18</v>
       </c>
@@ -3614,7 +3614,7 @@
         <v>0.35135135135135132</v>
       </c>
     </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>18</v>
       </c>
@@ -3670,7 +3670,7 @@
         <v>0.35135135135135132</v>
       </c>
     </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>18</v>
       </c>
@@ -3726,7 +3726,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>18</v>
       </c>
@@ -3782,7 +3782,7 @@
         <v>0.18918918918918909</v>
       </c>
     </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>18</v>
       </c>
@@ -3838,7 +3838,7 @@
         <v>0.18918918918918909</v>
       </c>
     </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>18</v>
       </c>
@@ -3894,7 +3894,7 @@
         <v>0.13513513513513509</v>
       </c>
     </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>18</v>
       </c>

</xml_diff>